<commit_message>
updated figures for Weka results and changed wording in paper
</commit_message>
<xml_diff>
--- a/ese/exp3-unsup-numbers.xlsx
+++ b/ese/exp3-unsup-numbers.xlsx
@@ -91,8 +91,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,8 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -524,7 +533,7 @@
       <c r="H2">
         <v>0.57303370786499996</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>0.65985018726599998</v>
       </c>
       <c r="J2">
@@ -562,7 +571,7 @@
       <c r="H3">
         <v>0.77777777777799995</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>0.548772609819</v>
       </c>
       <c r="J3">
@@ -600,7 +609,7 @@
       <c r="H4">
         <v>0.92682926829300005</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>0.65163302495099995</v>
       </c>
       <c r="J4">
@@ -638,7 +647,7 @@
       <c r="H5">
         <v>0.82352941176500005</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>0.66528583264300001</v>
       </c>
       <c r="J5">
@@ -676,7 +685,7 @@
       <c r="H6">
         <v>0.46250000000000002</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>0.56620145631100005</v>
       </c>
       <c r="J6">
@@ -714,7 +723,7 @@
       <c r="H7">
         <v>0.944444444444</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>0.59486373165600004</v>
       </c>
       <c r="J7">
@@ -752,7 +761,7 @@
       <c r="H8">
         <v>0.67100977198699996</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>0.56811465412399997</v>
       </c>
       <c r="J8">
@@ -769,6 +778,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
@@ -795,7 +805,7 @@
       <c r="H10">
         <v>0.32510288065800003</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>0.57363015753000002</v>
       </c>
       <c r="J10">
@@ -833,7 +843,7 @@
       <c r="H11">
         <v>0.72093023255800004</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>0.61921281425300001</v>
       </c>
       <c r="J11">
@@ -871,7 +881,7 @@
       <c r="H12">
         <v>0.70085470085500001</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <v>0.63081114573700003</v>
       </c>
       <c r="J12">
@@ -909,7 +919,7 @@
       <c r="H13">
         <v>0.64890282131699994</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>0.62033156047100002</v>
       </c>
       <c r="J13">
@@ -947,7 +957,7 @@
       <c r="H14">
         <v>0.16847826087000001</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>0.49841823491199999</v>
       </c>
       <c r="J14">
@@ -985,7 +995,7 @@
       <c r="H15">
         <v>0.6875</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="1">
         <v>0.51342509025299998</v>
       </c>
       <c r="J15">
@@ -1023,7 +1033,7 @@
       <c r="H16">
         <v>0.481876332623</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="1">
         <v>0.53283110657499999</v>
       </c>
       <c r="J16">
@@ -1040,6 +1050,7 @@
       <c r="A17" t="s">
         <v>9</v>
       </c>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
@@ -1066,7 +1077,7 @@
       <c r="H18">
         <v>0.92115384615399998</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>0.49807692307700002</v>
       </c>
       <c r="J18">
@@ -1104,7 +1115,7 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="1">
         <v>0.50601374570400004</v>
       </c>
       <c r="J19">
@@ -1142,7 +1153,7 @@
       <c r="H20">
         <v>0.96932515337400005</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="1">
         <v>0.49619297500999998</v>
       </c>
       <c r="J20">
@@ -1180,7 +1191,7 @@
       <c r="H21">
         <v>0.98840579710099996</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="1">
         <v>0.50776222058499998</v>
       </c>
       <c r="J21">
@@ -1218,7 +1229,7 @@
       <c r="H22">
         <v>0.79464285714299998</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="1">
         <v>0.49012445887400002</v>
       </c>
       <c r="J22">
@@ -1256,7 +1267,7 @@
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="1">
         <v>0.50245098039199998</v>
       </c>
       <c r="J23">
@@ -1294,7 +1305,7 @@
       <c r="H24">
         <v>0.94045676998399996</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="1">
         <v>0.49624215698899998</v>
       </c>
       <c r="J24">
@@ -1311,6 +1322,7 @@
       <c r="A25" t="s">
         <v>10</v>
       </c>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
@@ -1337,7 +1349,7 @@
       <c r="H26">
         <v>0.91037735849099999</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="1">
         <v>0.491403632516</v>
       </c>
       <c r="J26">
@@ -1375,7 +1387,7 @@
       <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="1">
         <v>0.50687622789800002</v>
       </c>
       <c r="J27">
@@ -1413,7 +1425,7 @@
       <c r="H28">
         <v>0.98675496688700004</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="1">
         <v>0.50769241186900005</v>
       </c>
       <c r="J28">
@@ -1451,7 +1463,7 @@
       <c r="H29">
         <v>0.98728813559299999</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="1">
         <v>0.504782681658</v>
       </c>
       <c r="J29">
@@ -1489,7 +1501,7 @@
       <c r="H30">
         <v>0.78571428571400004</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="1">
         <v>0.48429683157300002</v>
       </c>
       <c r="J30">
@@ -1527,7 +1539,7 @@
       <c r="H31">
         <v>1</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="1">
         <v>0.50315126050400005</v>
       </c>
       <c r="J31">
@@ -1565,7 +1577,7 @@
       <c r="H32">
         <v>0.95</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="1">
         <v>0.50301418439699996</v>
       </c>
       <c r="J32">

</xml_diff>